<commit_message>
updating BOM with purchases
</commit_message>
<xml_diff>
--- a/BOM food computer.xlsx
+++ b/BOM food computer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camille\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\DEV\FoodPC\gro-hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,13 +17,12 @@
     <sheet name="Kit" sheetId="3" r:id="rId3"/>
     <sheet name="Tools" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="188">
   <si>
     <t>Item Name</t>
   </si>
@@ -584,13 +583,16 @@
   </si>
   <si>
     <t>measure out fertilizers, yeast, and sugar</t>
+  </si>
+  <si>
+    <t>Ash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -685,8 +687,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -705,6 +714,11 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -715,10 +729,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -811,8 +826,10 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1091,13 +1108,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -1107,7 +1124,7 @@
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1127,7 +1144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1137,7 +1154,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/CyberPower-CSB606-Protector-6-Outlets-Joules/dp/B00FLTTGYG/ref=pd_sim_23_1?ie=UTF8&amp;refRID=163NC2W6A2KW7EF2RB9B","Power Strip")</f>
         <v>Power Strip</v>
@@ -1158,8 +1175,11 @@
         <f t="shared" ref="F3:F5" si="0">E3*D3</f>
         <v>10.15</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G3" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Switching-Power-Supply-Strip-Light/dp/B007MWNF5Q/ref=pd_sim_60_6?ie=UTF8&amp;refRID=0WA6QTYVKRWRGRG1ZKN2A","Main Power Supply")</f>
         <v>Main Power Supply</v>
@@ -1180,8 +1200,11 @@
         <f t="shared" si="0"/>
         <v>24.96</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G4" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0002J1KS0/ref=ox_sc_act_title_1?ie=UTF8&amp;psc=1&amp;smid=ATVPDKIKX0DER","AC Extension Cable")</f>
         <v>AC Extension Cable</v>
@@ -1202,8 +1225,11 @@
         <f t="shared" si="0"/>
         <v>4.99</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G5" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -1213,7 +1239,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/CanaKit-Raspberry-Power-Supply-Listed/dp/B00MARDJZ4/ref=sr_1_2?ie=UTF8&amp;qid=1439988175&amp;sr=8-2&amp;keywords=raspberry+pi+2+power+supply","Raspberry Pi Power Supply")</f>
         <v>Raspberry Pi Power Supply</v>
@@ -1234,8 +1260,11 @@
         <f t="shared" ref="F7:F10" si="1">E7*D7</f>
         <v>9.99</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G7" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Ximico-Arduino-Cable-Atmega2560-16au-Compatible/dp/B00KG3SBE8/ref=sr_1_2?s=pc&amp;ie=UTF8&amp;qid=1439935660&amp;sr=1-2&amp;keywords=arduino+mega","Arduino Mega 2560")</f>
         <v>Arduino Mega 2560</v>
@@ -1256,8 +1285,11 @@
         <f t="shared" si="1"/>
         <v>14.19</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G8" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Raspberry-Pi-Model-Desktop-Linux/dp/B00T2U7R7I","Raspberry Pi 2 Model B")</f>
         <v>Raspberry Pi 2 Model B</v>
@@ -1278,8 +1310,11 @@
         <f t="shared" si="1"/>
         <v>41.87</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G9" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Kingston-microSDHC-Memory-SDC4-8GBET/dp/B00200K1TS/ref=sr_1_8?s=pc&amp;ie=UTF8&amp;qid=1439988385&amp;sr=1-8&amp;keywords=micro+SD","Micro SD Card")</f>
         <v>Micro SD Card</v>
@@ -1300,8 +1335,11 @@
         <f t="shared" si="1"/>
         <v>3.99</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G10" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00EUHRLF6/ref=ox_sc_imb_mini_detail?ie=UTF8&amp;psc=1&amp;smid=A1DCPNQKKEISZB","Ethernet cable")</f>
         <v>Ethernet cable</v>
@@ -1319,8 +1357,11 @@
       <c r="F11" s="15">
         <v>5.99</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G11" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Gikfun-Protoshield-Prototype-Shield-Arduino/dp/B00Q9YBQ04/ref=sr_1_6?s=pc&amp;ie=UTF8&amp;qid=1439935499&amp;sr=1-6&amp;keywords=protoshield","Arduino Mega Protoshield")</f>
         <v>Arduino Mega Protoshield</v>
@@ -1341,8 +1382,11 @@
         <f t="shared" ref="F12:F15" si="2">E12*D12</f>
         <v>8.99</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="G12" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Base-Shield-V2-p-1378.html","Grove Base Shield")</f>
         <v>Grove Base Shield</v>
@@ -1364,7 +1408,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="str">
         <f>HYPERLINK("https://www.adafruit.com/products/2097","Touchscreen Display")</f>
         <v>Touchscreen Display</v>
@@ -1386,7 +1430,7 @@
         <v>44.95</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/ribbon-cable-Raspberry-stackable-header/dp/B00G84WNA2/ref=sr_1_1?ie=UTF8&amp;qid=1440708449&amp;sr=8-1&amp;keywords=raspberry+pi+cable","GPIO Cable ")</f>
         <v xml:space="preserve">GPIO Cable </v>
@@ -1408,7 +1452,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>71</v>
       </c>
@@ -1418,7 +1462,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/JBtek-Channel-Module-Arduino-Raspberry/dp/B00KTEN3TM/ref=sr_1_1?s=pc&amp;ie=UTF8&amp;qid=1439935182&amp;sr=1-1&amp;keywords=4+Channel+Relay","4-Channel Relay")</f>
         <v>4-Channel Relay</v>
@@ -1440,7 +1484,7 @@
         <v>13.96</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/52171-4E-Pre-Galvanized-Eccentric-Knockouts/dp/B000HEFCKC/ref=pd_bxgy_60_text_y","AC Relay Box Back Receptacle")</f>
         <v>AC Relay Box Back Receptacle</v>
@@ -1462,7 +1506,7 @@
         <v>2.04</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/RS8-Outlet-Surface-Square-Galvanized/dp/B000HEIU9W/ref=pd_sim_60_23?ie=UTF8&amp;refRID=0C95J370DWVEWW0H1MG8","AC Relay Box Front Panel")</f>
         <v>AC Relay Box Front Panel</v>
@@ -1484,7 +1528,7 @@
         <v>4.92</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Leviton-T5320-W-Resistant-Receptacle-Residential/dp/B0015R9M2Y/ref=pd_bxgy_60_img_z","AC Plug")</f>
         <v>AC Plug</v>
@@ -1505,8 +1549,11 @@
         <f t="shared" si="3"/>
         <v>2.38</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G20" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0002J1KS0/ref=ox_sc_act_title_1?ie=UTF8&amp;psc=1&amp;smid=ATVPDKIKX0DER","AC Extension Cable")</f>
         <v>AC Extension Cable</v>
@@ -1527,8 +1574,11 @@
         <f t="shared" si="3"/>
         <v>4.99</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G21" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>77</v>
       </c>
@@ -1538,7 +1588,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Triangle-Bulbs-T93007-Waterproof-Flexible/dp/B005EHHLD8/ref=sr_1_1?ie=UTF8&amp;qid=1443799060&amp;sr=8-1&amp;keywords=waterproof+led+strip","White LED Strip")</f>
         <v>White LED Strip</v>
@@ -1560,7 +1610,7 @@
         <v>19.98</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Erligpowht-Indoor-Garden-Plant-Hanging/dp/B00S2DPYQM/ref=sr_1_fkmr2_2?ie=UTF8&amp;qid=1443799150&amp;sr=8-2-fkmr2&amp;keywords=grow+led+panel+erwl","Grow LED Panel")</f>
         <v>Grow LED Panel</v>
@@ -1582,7 +1632,7 @@
         <v>75.98</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>80</v>
       </c>
@@ -1592,7 +1642,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/dp/B003XDTWN2/ref=sr_ph?&amp;ie=UTF8&amp;qid=1440085101&amp;sr=1&amp;keywords=heater","Heater")</f>
         <v>Heater</v>
@@ -1613,8 +1663,11 @@
         <f t="shared" ref="F26:F31" si="5">E26*D26</f>
         <v>15.99</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G26" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Acoustic-Audio-Tek%C2%A8Portable-Humidifier-travel--White/dp/B00RM5Z44S/ref=sr_1_4?s=home-garden&amp;ie=UTF8&amp;qid=1440427700&amp;sr=1-4&amp;keywords=bottle+cap+humidifier","Humidifier")</f>
         <v>Humidifier</v>
@@ -1635,8 +1688,11 @@
         <f t="shared" si="5"/>
         <v>7.35</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G27" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/dp/B00WJW3NM4/ref=twister_B00WJW3M3Y?_encoding=UTF8&amp;psc=1","USB Wall Adapter")</f>
         <v>USB Wall Adapter</v>
@@ -1658,7 +1714,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Bgears-b-Blaster-120mm-Bearing-Extreme/dp/B0043GKY1W/ref=sr_1_1?ie=UTF8&amp;qid=1440020490&amp;sr=8-1&amp;keywords=bgears+120mm","Circulation/Vent Fans")</f>
         <v>Circulation/Vent Fans</v>
@@ -1680,7 +1736,7 @@
         <v>25.86</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Tjernlund-1519003-Wire-Fan-Guard/dp/B008RMKFTO/ref=sr_1_2?ie=UTF8&amp;qid=1440019946&amp;sr=8-2&amp;keywords=fan+guard","Fan Guards")</f>
         <v>Fan Guards</v>
@@ -1702,7 +1758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Dundas-Jafine-LC4WZW-ProVent-4-Inches/dp/B0016487CC/ref=sr_1_3?ie=UTF8&amp;qid=1440020385&amp;sr=8-3&amp;keywords=Louvered+Vent+Cap","Fan Louvres")</f>
         <v>Fan Louvres</v>
@@ -1724,7 +1780,7 @@
         <v>13.68</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>87</v>
       </c>
@@ -1734,7 +1790,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="str">
         <f>HYPERLINK("http://www.co2meter.com/products/cozir-0-2-co2-sensor","CO2 Sensor")</f>
         <v>CO2 Sensor</v>
@@ -1756,7 +1812,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-TemperatureHumidity-Sensor-Pro-p-838.html","Air Temperature and Humidity Sensor")</f>
         <v>Air Temperature and Humidity Sensor</v>
@@ -1778,7 +1834,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-Digital-Light-Sensor-p-1281.html","Light Intensity Sensor")</f>
         <v>Light Intensity Sensor</v>
@@ -1800,7 +1856,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00YCDHQ8K?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o06_s00","Webcam")</f>
         <v>Webcam</v>
@@ -1822,7 +1878,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>93</v>
       </c>
@@ -1832,7 +1888,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0009SUF08?keywords=reed%20switch&amp;qid=1443805349&amp;ref_=sr_1_1&amp;sr=8-1","Magnetic Switch")</f>
         <v>Magnetic Switch</v>
@@ -1854,7 +1910,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Micro-Limit-Switch-Roller-Action/dp/B00E0JOTV8/ref=sr_1_1?s=lamps-light&amp;ie=UTF8&amp;qid=1443805532&amp;sr=1-1&amp;keywords=limit+switch","Limit Switch")</f>
         <v>Limit Switch</v>
@@ -1876,7 +1932,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>97</v>
       </c>
@@ -1886,7 +1942,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0009YJ4N6?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_1&amp;smid=ATVPDKIKX0DER","Air Pump")</f>
         <v>Air Pump</v>
@@ -1907,8 +1963,11 @@
         <f t="shared" ref="F41:F45" si="8">E41*D41</f>
         <v>9.3800000000000008</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G41" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Jardin-Aquarium-Ceramic-Diffusers-Diameter/dp/B0050HJ7Q6/ref=pd_bxgy_199_img_z","Air Stone")</f>
         <v>Air Stone</v>
@@ -1930,7 +1989,7 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Standard-Airline-Tubing-Accessories-25-Feet/dp/B0002563MW/ref=pd_bxgy_199_img_y","Air Pump Tubing")</f>
         <v>Air Pump Tubing</v>
@@ -1952,7 +2011,7 @@
         <v>4.04</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00EWENMAU?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_2&amp;smid=A14L9DIA3NK9B0","Aquarium Pump")</f>
         <v>Aquarium Pump</v>
@@ -1974,7 +2033,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0079QUTSQ?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_1&amp;smid=ATVPDKIKX0DER","Pump Tubing")</f>
         <v>Pump Tubing</v>
@@ -1996,7 +2055,7 @@
         <v>14.39</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>104</v>
       </c>
@@ -2006,7 +2065,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="str">
         <f>HYPERLINK("http://www.dfrobot.com/index.php?route=product/product&amp;product_id=1123&amp;search=DFR0300#.VdTDoFNViko","Water Temperature and EC Sensor")</f>
         <v>Water Temperature and EC Sensor</v>
@@ -2028,7 +2087,7 @@
         <v>69.900000000000006</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="str">
         <f>HYPERLINK("http://www.dfrobot.com/index.php?route=product/product&amp;product_id=1025#.Vg60SBNViko","pH Sensor")</f>
         <v>pH Sensor</v>
@@ -2050,7 +2109,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>108</v>
       </c>
@@ -2082,7 +2141,7 @@
         <v>19.989999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="19"/>
       <c r="B51" s="19"/>
       <c r="C51" s="19"/>
@@ -2090,7 +2149,7 @@
       <c r="E51" s="19"/>
       <c r="F51" s="19"/>
     </row>
-    <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>110</v>
       </c>
@@ -2122,7 +2181,7 @@
         <v>10.93</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Wago-222-412-222-413-Lever-Nut-Assortment/dp/B00U4520JK/ref=sr_1_1?ie=UTF8&amp;qid=1443798480&amp;sr=8-1&amp;keywords=wago+lever+nut+assortment","Wago Lever Nut Assortment")</f>
         <v>Wago Lever Nut Assortment</v>
@@ -2166,7 +2225,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-c-98_106_57/?ref=crumb","Grove Cables")</f>
         <v>Grove Cables</v>
@@ -2181,7 +2240,7 @@
       <c r="E56" s="19"/>
       <c r="F56" s="19"/>
     </row>
-    <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
       <c r="C57" s="8" t="s">
@@ -2191,7 +2250,7 @@
       <c r="E57" s="19"/>
       <c r="F57" s="19"/>
     </row>
-    <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="24" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/3M-Scotch-1-in-x-12-5-yds-Indoor-Outdoor-Mounting-Tape-411-LONG-DC/100153200","Foam mounting tape")</f>
         <v>Foam mounting tape</v>
@@ -2213,7 +2272,7 @@
         <v>15.97</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="24" t="str">
         <f>HYPERLINK("http://www.amazon.com/3M-Electrical-75-Inch-66-Foot-0085-Inch/dp/B00004WCCP/ref=sr_1_1?s=industrial&amp;ie=UTF8&amp;qid=1443807012&amp;sr=1-1&amp;keywords=electrical+tape","Electrical Tape")</f>
         <v>Electrical Tape</v>
@@ -2235,7 +2294,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="24" t="str">
         <f>HYPERLINK("http://www.digikey.com/product-search/en?KeyWords=377-2132-ND&amp;WT.z_header=search_go","Air Exchange Box")</f>
         <v>Air Exchange Box</v>
@@ -2279,7 +2338,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="24" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-8-x-2-in-Zinc-Plated-Pan-Head-Phillips-Drive-Sheet-Metal-Screw-50-Piece-801632/204275094","Long Screws")</f>
         <v>Long Screws</v>
@@ -2301,7 +2360,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>123</v>
       </c>

</xml_diff>